<commit_message>
Add data cleaning functionality for breath frequency analysis
- Introduced a new module for data cleaning with functions to normalize column names, convert time formats, correct data types, and rename columns.
- Implemented a function to load and process Excel files, handling multiple sheets and applying cleaning functions.
- Created an `__init__.py` file to facilitate module imports.
</commit_message>
<xml_diff>
--- a/ore_lavorate_calcolate.xlsx
+++ b/ore_lavorate_calcolate.xlsx
@@ -75,7 +75,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -83,11 +83,27 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="165" fontId="2" fillId="3" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="166" fontId="2" fillId="3" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -453,7 +469,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,8 +479,9 @@
   <cols>
     <col width="20" customWidth="1" min="1" max="1"/>
     <col width="20" customWidth="1" min="2" max="2"/>
-    <col width="15" customWidth="1" min="3" max="3"/>
-    <col width="15" customWidth="1" min="4" max="4"/>
+    <col width="10" customWidth="1" min="3" max="3"/>
+    <col width="10" customWidth="1" min="4" max="4"/>
+    <col width="30" customWidth="1" min="5" max="5"/>
     <col width="15" customWidth="1" min="7" max="7"/>
     <col width="15" customWidth="1" min="8" max="8"/>
     <col width="15" customWidth="1" min="9" max="9"/>
@@ -473,27 +490,27 @@
     <row r="1">
       <c r="A1" s="2" t="inlineStr">
         <is>
-          <t>start</t>
+          <t>Start Time</t>
         </is>
       </c>
       <c r="B1" s="2" t="inlineStr">
         <is>
-          <t>end</t>
+          <t>End Time</t>
         </is>
       </c>
       <c r="C1" s="2" t="inlineStr">
         <is>
-          <t>note</t>
+          <t>Duration (hrs)</t>
         </is>
       </c>
       <c r="D1" s="2" t="inlineStr">
         <is>
-          <t>duration_hrs</t>
+          <t>Cost (€)</t>
         </is>
       </c>
       <c r="E1" s="2" t="inlineStr">
         <is>
-          <t>cost_eur</t>
+          <t>Note</t>
         </is>
       </c>
       <c r="G1" s="3" t="n"/>
@@ -515,29 +532,48 @@
       <c r="B2" s="5" t="n">
         <v>46060.93055555555</v>
       </c>
-      <c r="C2" s="6" t="inlineStr">
+      <c r="C2" s="6" t="n">
+        <v>1.666666666666667</v>
+      </c>
+      <c r="D2" s="7" t="n">
+        <v>41.66666666666667</v>
+      </c>
+      <c r="E2" s="8" t="inlineStr">
         <is>
           <t>Data Cleaning, ho cercato di far quadrare l'excel</t>
         </is>
       </c>
-      <c r="D2" s="7" t="n">
-        <v>1.666666666666667</v>
-      </c>
-      <c r="E2" s="3" t="n">
-        <v>41.66666666666667</v>
-      </c>
-      <c r="G2" s="4" t="inlineStr">
+      <c r="G2" s="9" t="inlineStr">
         <is>
           <t>TOTAL DUE:</t>
         </is>
       </c>
-      <c r="H2" s="8">
-        <f>SUM(D2:D2)</f>
+      <c r="H2" s="10">
+        <f>SUM(C2:C3)</f>
         <v/>
       </c>
-      <c r="I2" s="9">
-        <f>SUM(E2:E2)</f>
+      <c r="I2" s="11">
+        <f>SUM(D2:D3)</f>
         <v/>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="5" t="n">
+        <v>46061.56944444445</v>
+      </c>
+      <c r="B3" s="5" t="n">
+        <v>46061.59930555556</v>
+      </c>
+      <c r="C3" s="6" t="n">
+        <v>0.7166666666666667</v>
+      </c>
+      <c r="D3" s="7" t="n">
+        <v>17.91666666666667</v>
+      </c>
+      <c r="E3" s="8" t="inlineStr">
+        <is>
+          <t>Refactored the cleaning code</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>